<commit_message>
Website V1.0.0 240625 Upgrade GPT settings to Alert Must Act & SOFR Alert
</commit_message>
<xml_diff>
--- a/gptSettings/gptSettings.xlsx
+++ b/gptSettings/gptSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InfiniteWisdom\gptSettings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406B8A55-2A29-4832-BEEC-AE04D95CC1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD0989E-B0AC-424E-9E3A-4CCC7866E521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,11 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">以下是報告所需要根據的FED關鍵數據:
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>finalText</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,13 +139,17 @@
   <si>
     <t xml:space="preserve">請整合3天泡沫分數的數據，FED關鍵數據與3天內的新聞，用繁體中文，寫出一份人看得懂且內容豐富的每日投資報告
 請嚴格根據泡沫分數裡面有的標的，進行報告的撰寫
-根據過去3天的泡沫數據，分析各投資商品的泡沫機率變化趨勢，並比對FED關鍵數據與3天的新聞內容，提供實用的投資建議。
-如果有需要，請確認有符合貨幣銀行經濟，總體經濟，微觀經濟理論，行為經濟理論，現在貨幣理論，等等最新經濟理論，必要時幫忙用現代經濟學的觀點補充說明看到的現象
-對於泡沫機率持續上升且遠大於0.5的商品，如果 ”新聞現況” 支持，建議投資者考慮賣出，以避免未來價格下跌時的損失，想辦法用新聞觀點說服使用者賣出。
-對於泡沫機率下降遠小於0.5的商品，如果 ”新聞現況” 支持，可以考慮作為買入選項，想辦法用新聞觀點說服使用者買入。
-對於泡沫分數0.5左右的部分，建議觀望不要有任何動作。
-請逐步仔細推導不同商品之間泡沫的關係用以形成論點，整理支持這些論點的新聞，用高度專業投資人的角度來給出結果
-最後，我們提醒投資者注意市場風險，特別是對於泡沫機率高的商品，應該謹慎進行投資決策。
+根據過去3天的泡沫數據，分析各投資商品的泡沫機率變化趨勢，並比對FED關鍵數據與3天的新聞內容，提供實用的投資建議
+請確認有符合貨幣銀行經濟，總體經濟，微觀經濟理論，行為經濟理論，現在貨幣理論，等等最新經濟理論，必要時幫忙用現代經濟學的觀點補充說明看到的現象
+對於泡沫機率持續上升且遠大於0.5的商品，如果 ”新聞現況” 支持，建議投資者考慮賣出，以避免未來價格下跌時的損失，想辦法用新聞觀點與相關經濟數據，說服使用者賣出
+對於泡沫機率持續下降且遠小於0.5的商品，如果 ”新聞現況” 支持，可以考慮作為買入選項，想辦法用新聞觀點與相關經濟數據說服使用者買入
+對於以上泡沫機率持續上升且遠大於0.5的商品，或泡沫機率持續下降且遠小於0.5的商品，如果出現以下兩種情況:
+泡沫機率D1相較於D7 &amp; D14 &amp; D30如果出現大幅下降”強烈建議”買入建立投資部位
+泡沫機率D1相較於D7 &amp; D14 &amp; D30如果出現大幅上升”強烈建議”賣出投資部位避險
+對於泡沫分數0.45 ~ 0.55的商品，建議觀望不要有任何動作
+如果看到 SOFR &gt; (FED Fund Rate + 0.2)，請務必警告所有高泡沫資產，因海外美元吃緊，即將面臨大幅度下跌的風險 (被提款成美元用來滿足流動性需求)
+請逐步仔細推導不同商品之間泡沫的關係用以形成論點，整理支持這些論點的新聞與相關經濟數據，用高度專業投資人的角度來給出結果
+最後，我們提醒投資者注意市場風險，特別是對於泡沫機率高的商品，應該謹慎進行投資決策
 請不要洩漏任何關於泡沫分數的技術細節
 以下回答格式僅作參考，請根據後續給予的資料製作報告，分析資產類別請盡量帶到此時所有關鍵的投資類別
 ## 投資商品泡沫分析
@@ -188,10 +187,15 @@
   ...
 ## 風險提示
 投資有風險，市場總是充滿不確定性。我們的建議僅供參考，投資者應根據自身的風險承受能力和投資目標，做出獨立的投資決策。
-以下皆是用來產生報告的原始資料
+以下皆是用來產生報告的原始資料:
 以下是各種投資商品的買賣未來一年預測(泡沫分數)，該技術使用Transformer，針對過去2000天以上的資料做RL強化學習
 結果為分析，在一年到期時，越接近0買的勝率越高 (到期時預期價格比買入高)，越接近1賣的勝率越高 (到期時預期價格比此時賣出低)，可看成越接近1，資產價格泡沫的機率越高，預測未來半年到1年的泡沫機率，D1是過去一天的預期，D7是過去七天的平均預期，
 PP80是當日有80%機率成交率的價格，如果是偏買就是低掛價，如果是偏賣，就是高掛價，PP100就是當日價格，可以直接成交
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">以下是報告所需要根據的FED經濟關鍵數據:
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -526,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -549,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
@@ -557,79 +561,79 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Website V1.0.0 240626 Upgrade GPT settings to Alert Must Act & SOFR Alert
</commit_message>
<xml_diff>
--- a/gptSettings/gptSettings.xlsx
+++ b/gptSettings/gptSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InfiniteWisdom\gptSettings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A05C6F4-6479-4B9A-8E21-8B61DAFCDB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F24BA17-D70E-440D-8391-B9AD79AC5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1275" windowWidth="26235" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -145,14 +145,13 @@
     <t xml:space="preserve">請整合3天泡沫分數的數據，FED關鍵數據與3天內的新聞，用繁體中文，寫出一份人看得懂且內容豐富的每日投資報告
 請嚴格根據泡沫分數裡面有的標的，進行報告的撰寫
 根據過去3天的泡沫數據，分析各投資商品的泡沫機率變化趨勢，並比對FED關鍵數據與3天的新聞內容，提供實用的投資建議
-請確認有符合貨幣銀行經濟，總體經濟，微觀經濟理論，行為經濟理論，現在貨幣理論，等等最新經濟理論，必要時幫忙用現代經濟學的觀點補充說明看到的現象
+如果看到 SOFR &gt; (FED Fund Rate + 0.2)，所有高泡沫資產，因海外美元吃緊，即將面臨大幅度下跌的風險 (被提款成美元用來滿足流動性需求)
 對於泡沫機率持續上升且遠大於0.5的商品，如果 ”新聞現況” 支持，建議投資者考慮賣出，以避免未來價格下跌時的損失，想辦法用新聞觀點與相關經濟數據，說服使用者賣出
 對於泡沫機率持續下降且遠小於0.5的商品，如果 ”新聞現況” 支持，可以考慮作為買入選項，想辦法用新聞觀點與相關經濟數據說服使用者買入
 對於以上泡沫機率持續上升且遠大於0.5的商品，或泡沫機率持續下降且遠小於0.5的商品，如果出現以下兩種情況:
 泡沫機率D1相較於D7 &amp; D14 &amp; D30，如果出現大幅下降”強烈建議”買入建立投資部位
 泡沫機率D1相較於D7 &amp; D14 &amp; D30，如果出現大幅上升”強烈建議”賣出投資部位避險
 對於泡沫分數0.45 ~ 0.55的商品，建議觀望不要有任何動作
-如果看到 SOFR &gt; (FED Fund Rate + 0.2)，請務必警告所有高泡沫資產，因海外美元吃緊，即將面臨大幅度下跌的風險 (被提款成美元用來滿足流動性需求)
 請逐步仔細推導不同商品之間泡沫的關係用以形成論點，整理支持這些論點的新聞與相關經濟數據，用高度專業投資人的角度來給出結果
 最後，我們提醒投資者注意市場風險，特別是對於泡沫機率高的商品，應該謹慎進行投資決策
 請不要洩漏任何關於泡沫分數的技術細節

</xml_diff>